<commit_message>
Começo da estilização da home page
</commit_message>
<xml_diff>
--- a/docs/Backlog.xlsx
+++ b/docs/Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Documents\Bandtec\PI\Projeto_Individual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Documents\Bandtec\PI\Projeto_Individual\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7121BE3-53E6-4856-8215-23E867D7DEF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675B0E1E-6F39-448F-9369-3FC39CCBF5BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="2640" windowWidth="15375" windowHeight="7875" xr2:uid="{35D73CA7-2B52-48EB-B275-714EC7D34A39}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1">
         <v>21</v>
@@ -598,7 +598,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>8</v>

</xml_diff>